<commit_message>
added 09-2017 salary data to archive
</commit_message>
<xml_diff>
--- a/archive/salary-data/salary - paste new data here.xlsx
+++ b/archive/salary-data/salary - paste new data here.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sba\SBA-white\archive\salary-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15885" windowHeight="10695" activeTab="1"/>
   </bookViews>
@@ -403,8 +408,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -797,17 +802,17 @@
     <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="23" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -817,6 +822,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -863,7 +876,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -895,9 +908,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -929,6 +943,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -1104,7 +1119,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1114,44 +1129,44 @@
       <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="51" max="51" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="44.25" customHeight="1">
-      <c r="A2" s="55" t="s">
+    <row r="2" spans="1:54" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
     </row>
-    <row r="4" spans="1:54">
-      <c r="A4" s="54">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A4" s="56">
         <v>2013</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
@@ -1205,7 +1220,7 @@
       <c r="BA4" s="33"/>
       <c r="BB4" s="33"/>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="B5" s="37" t="s">
         <v>0</v>
@@ -1367,7 +1382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1531,7 +1546,7 @@
         <v>40228.930790920516</v>
       </c>
     </row>
-    <row r="7" spans="1:54">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>9</v>
       </c>
@@ -1695,7 +1710,7 @@
         <v>49144.265686748615</v>
       </c>
     </row>
-    <row r="8" spans="1:54">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1859,7 +1874,7 @@
         <v>29050.158726926027</v>
       </c>
     </row>
-    <row r="9" spans="1:54">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -2023,7 +2038,7 @@
         <v>25192.402259839742</v>
       </c>
     </row>
-    <row r="10" spans="1:54" ht="16.5" customHeight="1">
+    <row r="10" spans="1:54" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -2187,7 +2202,7 @@
         <v>27798.617506103659</v>
       </c>
     </row>
-    <row r="11" spans="1:54">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -2351,7 +2366,7 @@
         <v>28143.74207004032</v>
       </c>
     </row>
-    <row r="12" spans="1:54">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -2515,7 +2530,7 @@
         <v>23239.310800577918</v>
       </c>
     </row>
-    <row r="13" spans="1:54">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -2679,7 +2694,7 @@
         <v>33191.240114403292</v>
       </c>
     </row>
-    <row r="14" spans="1:54">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -2843,7 +2858,7 @@
         <v>23730.388995209778</v>
       </c>
     </row>
-    <row r="15" spans="1:54">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -3007,7 +3022,7 @@
         <v>27145.923338717384</v>
       </c>
     </row>
-    <row r="16" spans="1:54">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -3171,7 +3186,7 @@
         <v>28153.052455166726</v>
       </c>
     </row>
-    <row r="17" spans="1:54">
+    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>99</v>
       </c>
@@ -3335,7 +3350,7 @@
         <v>46479.453987895853</v>
       </c>
     </row>
-    <row r="18" spans="1:54">
+    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -3499,7 +3514,7 @@
         <v>24952.473850869548</v>
       </c>
     </row>
-    <row r="19" spans="1:54">
+    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -3663,7 +3678,7 @@
         <v>30909.911403073944</v>
       </c>
     </row>
-    <row r="20" spans="1:54">
+    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -3827,7 +3842,7 @@
         <v>26144.953556607848</v>
       </c>
     </row>
-    <row r="21" spans="1:54">
+    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -3991,7 +4006,7 @@
         <v>25299.825539030266</v>
       </c>
     </row>
-    <row r="22" spans="1:54">
+    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -4155,7 +4170,7 @@
         <v>27704.16397870623</v>
       </c>
     </row>
-    <row r="23" spans="1:54">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -4319,7 +4334,7 @@
         <v>31039.746984540296</v>
       </c>
     </row>
-    <row r="24" spans="1:54">
+    <row r="24" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -4483,7 +4498,7 @@
         <v>31069.218104372274</v>
       </c>
     </row>
-    <row r="25" spans="1:54">
+    <row r="25" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>93</v>
       </c>
@@ -4647,7 +4662,7 @@
         <v>76916.37314439725</v>
       </c>
     </row>
-    <row r="26" spans="1:54">
+    <row r="26" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
         <v>26</v>
       </c>
@@ -4811,7 +4826,7 @@
         <v>44628.190599534108</v>
       </c>
     </row>
-    <row r="27" spans="1:54">
+    <row r="27" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -4975,7 +4990,7 @@
         <v>35264.912704266826</v>
       </c>
     </row>
-    <row r="28" spans="1:54">
+    <row r="28" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -5139,7 +5154,7 @@
         <v>49613.28561296931</v>
       </c>
     </row>
-    <row r="29" spans="1:54">
+    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -5303,7 +5318,7 @@
         <v>46123.324995913681</v>
       </c>
     </row>
-    <row r="30" spans="1:54">
+    <row r="30" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>94</v>
       </c>
@@ -5467,7 +5482,7 @@
         <v>84417.983001376619</v>
       </c>
     </row>
-    <row r="31" spans="1:54">
+    <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>106</v>
       </c>
@@ -5631,7 +5646,7 @@
         <v>42972.794628476404</v>
       </c>
     </row>
-    <row r="32" spans="1:54">
+    <row r="32" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -5795,7 +5810,7 @@
         <v>31055.483975470459</v>
       </c>
     </row>
-    <row r="33" spans="1:54">
+    <row r="33" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -5959,7 +5974,7 @@
         <v>31157.079751032612</v>
       </c>
     </row>
-    <row r="34" spans="1:54">
+    <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -6123,7 +6138,7 @@
         <v>38795.566787477081</v>
       </c>
     </row>
-    <row r="35" spans="1:54">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -6287,7 +6302,7 @@
         <v>56704.402775866198</v>
       </c>
     </row>
-    <row r="36" spans="1:54">
+    <row r="36" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -6451,7 +6466,7 @@
         <v>29380.257664137305</v>
       </c>
     </row>
-    <row r="37" spans="1:54">
+    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -6615,7 +6630,7 @@
         <v>24330.602452640145</v>
       </c>
     </row>
-    <row r="38" spans="1:54">
+    <row r="38" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -6779,7 +6794,7 @@
         <v>52269.405080487537</v>
       </c>
     </row>
-    <row r="39" spans="1:54">
+    <row r="39" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>108</v>
       </c>
@@ -6943,7 +6958,7 @@
         <v>28984.655429838291</v>
       </c>
     </row>
-    <row r="40" spans="1:54">
+    <row r="40" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>37</v>
       </c>
@@ -7107,7 +7122,7 @@
         <v>24773.005620148619</v>
       </c>
     </row>
-    <row r="41" spans="1:54">
+    <row r="41" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>38</v>
       </c>
@@ -7271,7 +7286,7 @@
         <v>24550.862695954635</v>
       </c>
     </row>
-    <row r="42" spans="1:54">
+    <row r="42" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>104</v>
       </c>
@@ -7387,7 +7402,7 @@
         <v>26322.917905137339</v>
       </c>
     </row>
-    <row r="43" spans="1:54">
+    <row r="43" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>39</v>
       </c>
@@ -7551,7 +7566,7 @@
         <v>31297.373997167593</v>
       </c>
     </row>
-    <row r="44" spans="1:54">
+    <row r="44" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>40</v>
       </c>
@@ -7715,7 +7730,7 @@
         <v>28013.319871262709</v>
       </c>
     </row>
-    <row r="45" spans="1:54">
+    <row r="45" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>41</v>
       </c>
@@ -7879,7 +7894,7 @@
         <v>28620.572560871165</v>
       </c>
     </row>
-    <row r="46" spans="1:54">
+    <row r="46" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>42</v>
       </c>
@@ -8043,7 +8058,7 @@
         <v>28255.942974566231</v>
       </c>
     </row>
-    <row r="47" spans="1:54">
+    <row r="47" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>105</v>
       </c>
@@ -8159,7 +8174,7 @@
         <v>25651.784032656538</v>
       </c>
     </row>
-    <row r="48" spans="1:54">
+    <row r="48" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A48" s="43" t="s">
         <v>43</v>
       </c>
@@ -8323,7 +8338,7 @@
         <v>23980.122178436392</v>
       </c>
     </row>
-    <row r="49" spans="1:54">
+    <row r="49" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>44</v>
       </c>
@@ -8487,7 +8502,7 @@
         <v>22382.716464128243</v>
       </c>
     </row>
-    <row r="50" spans="1:54">
+    <row r="50" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>45</v>
       </c>
@@ -8651,7 +8666,7 @@
         <v>22759.53240639151</v>
       </c>
     </row>
-    <row r="51" spans="1:54">
+    <row r="51" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>46</v>
       </c>
@@ -8815,7 +8830,7 @@
         <v>21219.350840175441</v>
       </c>
     </row>
-    <row r="52" spans="1:54">
+    <row r="52" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>47</v>
       </c>
@@ -8979,7 +8994,7 @@
         <v>22836.307281251131</v>
       </c>
     </row>
-    <row r="53" spans="1:54">
+    <row r="53" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>48</v>
       </c>
@@ -9143,7 +9158,7 @@
         <v>23598.111393491828</v>
       </c>
     </row>
-    <row r="54" spans="1:54">
+    <row r="54" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>49</v>
       </c>
@@ -9307,7 +9322,7 @@
         <v>22873.65337707445</v>
       </c>
     </row>
-    <row r="55" spans="1:54">
+    <row r="55" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>50</v>
       </c>
@@ -9471,7 +9486,7 @@
         <v>25990.726407639901</v>
       </c>
     </row>
-    <row r="56" spans="1:54" ht="17.25" customHeight="1">
+    <row r="56" spans="1:54" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="43" t="s">
         <v>92</v>
       </c>
@@ -9635,7 +9650,7 @@
         <v>30135.323987000811</v>
       </c>
     </row>
-    <row r="57" spans="1:54">
+    <row r="57" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
@@ -9799,7 +9814,7 @@
         <v>31982.674714937031</v>
       </c>
     </row>
-    <row r="58" spans="1:54">
+    <row r="58" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>52</v>
       </c>
@@ -9963,7 +9978,7 @@
         <v>28831.50027179551</v>
       </c>
     </row>
-    <row r="59" spans="1:54">
+    <row r="59" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>53</v>
       </c>
@@ -10127,7 +10142,7 @@
         <v>24726.518144210622</v>
       </c>
     </row>
-    <row r="60" spans="1:54">
+    <row r="60" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>54</v>
       </c>
@@ -10291,7 +10306,7 @@
         <v>33376.791867937573</v>
       </c>
     </row>
-    <row r="61" spans="1:54">
+    <row r="61" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>55</v>
       </c>
@@ -10455,7 +10470,7 @@
         <v>30133.612635619738</v>
       </c>
     </row>
-    <row r="62" spans="1:54">
+    <row r="62" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>56</v>
       </c>
@@ -10619,7 +10634,7 @@
         <v>24743.448635262757</v>
       </c>
     </row>
-    <row r="63" spans="1:54">
+    <row r="63" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>57</v>
       </c>
@@ -10783,7 +10798,7 @@
         <v>32767.432414290754</v>
       </c>
     </row>
-    <row r="64" spans="1:54">
+    <row r="64" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>58</v>
       </c>
@@ -10947,7 +10962,7 @@
         <v>24899.786439222935</v>
       </c>
     </row>
-    <row r="65" spans="1:54">
+    <row r="65" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>59</v>
       </c>
@@ -11111,7 +11126,7 @@
         <v>30864.958277951737</v>
       </c>
     </row>
-    <row r="66" spans="1:54">
+    <row r="66" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>60</v>
       </c>
@@ -11275,7 +11290,7 @@
         <v>29285.458798034837</v>
       </c>
     </row>
-    <row r="67" spans="1:54">
+    <row r="67" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>61</v>
       </c>
@@ -11439,7 +11454,7 @@
         <v>27046.929158461433</v>
       </c>
     </row>
-    <row r="68" spans="1:54">
+    <row r="68" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>62</v>
       </c>
@@ -11603,7 +11618,7 @@
         <v>32259.986146209067</v>
       </c>
     </row>
-    <row r="69" spans="1:54">
+    <row r="69" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>63</v>
       </c>
@@ -11767,7 +11782,7 @@
         <v>25069.776674149522</v>
       </c>
     </row>
-    <row r="70" spans="1:54">
+    <row r="70" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>64</v>
       </c>
@@ -11931,7 +11946,7 @@
         <v>26254.790438381904</v>
       </c>
     </row>
-    <row r="71" spans="1:54">
+    <row r="71" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A71" s="43" t="s">
         <v>95</v>
       </c>
@@ -12095,7 +12110,7 @@
         <v>47840.247801881793</v>
       </c>
     </row>
-    <row r="72" spans="1:54">
+    <row r="72" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>65</v>
       </c>
@@ -12259,7 +12274,7 @@
         <v>26561.481176677411</v>
       </c>
     </row>
-    <row r="73" spans="1:54">
+    <row r="73" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>66</v>
       </c>
@@ -12423,7 +12438,7 @@
         <v>35984.7743034753</v>
       </c>
     </row>
-    <row r="74" spans="1:54">
+    <row r="74" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>67</v>
       </c>
@@ -12587,7 +12602,7 @@
         <v>72097.26554480374</v>
       </c>
     </row>
-    <row r="75" spans="1:54">
+    <row r="75" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>100</v>
       </c>
@@ -12644,7 +12659,7 @@
       <c r="BA75" s="32"/>
       <c r="BB75" s="32"/>
     </row>
-    <row r="76" spans="1:54">
+    <row r="76" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>96</v>
       </c>
@@ -12808,7 +12823,7 @@
         <v>74859.536050178853</v>
       </c>
     </row>
-    <row r="77" spans="1:54">
+    <row r="77" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>97</v>
       </c>
@@ -12972,7 +12987,7 @@
         <v>105414.11581257809</v>
       </c>
     </row>
-    <row r="78" spans="1:54">
+    <row r="78" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>107</v>
       </c>
@@ -13136,7 +13151,7 @@
         <v>43601.523027458599</v>
       </c>
     </row>
-    <row r="79" spans="1:54">
+    <row r="79" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>68</v>
       </c>
@@ -13300,7 +13315,7 @@
         <v>32726.729288669299</v>
       </c>
     </row>
-    <row r="80" spans="1:54">
+    <row r="80" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A80" s="43" t="s">
         <v>98</v>
       </c>
@@ -13464,7 +13479,7 @@
         <v>35076.459671957593</v>
       </c>
     </row>
-    <row r="81" spans="1:54">
+    <row r="81" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>69</v>
       </c>
@@ -13628,7 +13643,7 @@
         <v>26930.128984881208</v>
       </c>
     </row>
-    <row r="82" spans="1:54">
+    <row r="82" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>70</v>
       </c>
@@ -13792,7 +13807,7 @@
         <v>32048.76956765963</v>
       </c>
     </row>
-    <row r="83" spans="1:54">
+    <row r="83" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>71</v>
       </c>
@@ -13956,7 +13971,7 @@
         <v>33608.89850803477</v>
       </c>
     </row>
-    <row r="84" spans="1:54">
+    <row r="84" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>72</v>
       </c>
@@ -14120,7 +14135,7 @@
         <v>34701.323923599492</v>
       </c>
     </row>
-    <row r="85" spans="1:54">
+    <row r="85" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>73</v>
       </c>
@@ -14284,7 +14299,7 @@
         <v>22503.840954751162</v>
       </c>
     </row>
-    <row r="86" spans="1:54">
+    <row r="86" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>74</v>
       </c>
@@ -14448,7 +14463,7 @@
         <v>34904.879933233475</v>
       </c>
     </row>
-    <row r="87" spans="1:54">
+    <row r="87" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>75</v>
       </c>
@@ -14612,7 +14627,7 @@
         <v>42610.08852592991</v>
       </c>
     </row>
-    <row r="88" spans="1:54">
+    <row r="88" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>76</v>
       </c>
@@ -14776,7 +14791,7 @@
         <v>40527.592362838921</v>
       </c>
     </row>
-    <row r="89" spans="1:54">
+    <row r="89" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>77</v>
       </c>
@@ -14940,7 +14955,7 @@
         <v>33700.546045289797</v>
       </c>
     </row>
-    <row r="90" spans="1:54">
+    <row r="90" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>78</v>
       </c>
@@ -15104,7 +15119,7 @@
         <v>33417.030856990175</v>
       </c>
     </row>
-    <row r="91" spans="1:54">
+    <row r="91" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>79</v>
       </c>
@@ -15268,7 +15283,7 @@
         <v>30914.225721762774</v>
       </c>
     </row>
-    <row r="92" spans="1:54">
+    <row r="92" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>80</v>
       </c>
@@ -15432,7 +15447,7 @@
         <v>43232.331744922565</v>
       </c>
     </row>
-    <row r="93" spans="1:54">
+    <row r="93" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A93" s="43" t="s">
         <v>81</v>
       </c>
@@ -15596,7 +15611,7 @@
         <v>52942.920228562136</v>
       </c>
     </row>
-    <row r="94" spans="1:54">
+    <row r="94" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>82</v>
       </c>
@@ -15760,7 +15775,7 @@
         <v>68590.068770599188</v>
       </c>
     </row>
-    <row r="95" spans="1:54">
+    <row r="95" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>83</v>
       </c>
@@ -15924,7 +15939,7 @@
         <v>77043.251535660063</v>
       </c>
     </row>
-    <row r="96" spans="1:54">
+    <row r="96" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>84</v>
       </c>
@@ -16088,7 +16103,7 @@
         <v>38986.146997387259</v>
       </c>
     </row>
-    <row r="97" spans="1:54">
+    <row r="97" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>85</v>
       </c>
@@ -16252,7 +16267,7 @@
         <v>49014.703383520296</v>
       </c>
     </row>
-    <row r="98" spans="1:54">
+    <row r="98" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>86</v>
       </c>
@@ -16416,7 +16431,7 @@
         <v>37521.953675837278</v>
       </c>
     </row>
-    <row r="99" spans="1:54">
+    <row r="99" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>87</v>
       </c>
@@ -16580,7 +16595,7 @@
         <v>79958.651157946748</v>
       </c>
     </row>
-    <row r="100" spans="1:54">
+    <row r="100" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>88</v>
       </c>
@@ -16744,7 +16759,7 @@
         <v>70052.393772833093</v>
       </c>
     </row>
-    <row r="101" spans="1:54">
+    <row r="101" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>89</v>
       </c>
@@ -16908,7 +16923,7 @@
         <v>35517.898455346483</v>
       </c>
     </row>
-    <row r="102" spans="1:54">
+    <row r="102" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>90</v>
       </c>
@@ -17072,12 +17087,12 @@
         <v>94997.137640590634</v>
       </c>
     </row>
-    <row r="104" spans="1:54" ht="34.5">
+    <row r="104" spans="1:54" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A104" s="26" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="105" spans="1:54" ht="17.25">
+    <row r="105" spans="1:54" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A105" s="25"/>
     </row>
   </sheetData>
@@ -17092,54 +17107,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BD93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="AM70" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="AM6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BC5" sqref="BC5:BC90"/>
+      <selection pane="bottomRight" activeCell="BD6" sqref="BD6:BD90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" customWidth="1"/>
     <col min="51" max="51" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="44.25" customHeight="1">
-      <c r="A2" s="55" t="s">
+    <row r="2" spans="1:56" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
     </row>
-    <row r="4" spans="1:55">
-      <c r="A4" s="54">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A4" s="56">
         <v>2013</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
@@ -17193,7 +17208,7 @@
       <c r="BA4" s="33"/>
       <c r="BB4" s="33"/>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="B5" s="37" t="s">
         <v>0</v>
@@ -17354,11 +17369,11 @@
       <c r="BB5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="BC5" s="57" t="s">
+      <c r="BC5" s="55" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:55">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -17521,11 +17536,14 @@
       <c r="BB6" s="28">
         <v>29050.158726926027</v>
       </c>
-      <c r="BC6" s="56">
+      <c r="BC6" s="54">
         <v>29370.977124008034</v>
       </c>
+      <c r="BD6" s="54">
+        <v>29089.721864473649</v>
+      </c>
     </row>
-    <row r="7" spans="1:55">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -17688,11 +17706,14 @@
       <c r="BB7" s="28">
         <v>25192.402259839742</v>
       </c>
-      <c r="BC7" s="56">
+      <c r="BC7" s="54">
         <v>24041.991820255789</v>
       </c>
+      <c r="BD7" s="54">
+        <v>24244.125516434455</v>
+      </c>
     </row>
-    <row r="8" spans="1:55" ht="16.5" customHeight="1">
+    <row r="8" spans="1:56" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -17855,11 +17876,14 @@
       <c r="BB8" s="28">
         <v>27798.617506103659</v>
       </c>
-      <c r="BC8" s="56">
+      <c r="BC8" s="54">
         <v>27594.660344784254</v>
       </c>
+      <c r="BD8" s="54">
+        <v>27880.748106309577</v>
+      </c>
     </row>
-    <row r="9" spans="1:55">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -18022,11 +18046,14 @@
       <c r="BB9" s="28">
         <v>28143.74207004032</v>
       </c>
-      <c r="BC9" s="56">
+      <c r="BC9" s="54">
         <v>27625.650029431694</v>
       </c>
+      <c r="BD9" s="54">
+        <v>27939.968191792585</v>
+      </c>
     </row>
-    <row r="10" spans="1:55">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -18189,11 +18216,14 @@
       <c r="BB10" s="28">
         <v>23239.310800577918</v>
       </c>
-      <c r="BC10" s="56">
+      <c r="BC10" s="54">
         <v>21859.998925110871</v>
       </c>
+      <c r="BD10" s="54">
+        <v>23210.414677174391</v>
+      </c>
     </row>
-    <row r="11" spans="1:55">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -18356,11 +18386,14 @@
       <c r="BB11" s="28">
         <v>33191.240114403292</v>
       </c>
-      <c r="BC11" s="56">
+      <c r="BC11" s="54">
         <v>33545.117041489895</v>
       </c>
+      <c r="BD11" s="54">
+        <v>33840.165326669732</v>
+      </c>
     </row>
-    <row r="12" spans="1:55">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -18523,11 +18556,14 @@
       <c r="BB12" s="28">
         <v>23730.388995209778</v>
       </c>
-      <c r="BC12" s="56">
+      <c r="BC12" s="54">
         <v>23350.962517433574</v>
       </c>
+      <c r="BD12" s="54">
+        <v>23593.056466563776</v>
+      </c>
     </row>
-    <row r="13" spans="1:55">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -18690,11 +18726,14 @@
       <c r="BB13" s="28">
         <v>27145.923338717384</v>
       </c>
-      <c r="BC13" s="56">
+      <c r="BC13" s="54">
         <v>26310.113112333096</v>
       </c>
+      <c r="BD13" s="54">
+        <v>27050.648666277299</v>
+      </c>
     </row>
-    <row r="14" spans="1:55">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -18857,11 +18896,14 @@
       <c r="BB14" s="28">
         <v>28153.052455166726</v>
       </c>
-      <c r="BC14" s="56">
+      <c r="BC14" s="54">
         <v>27224.656931975325</v>
       </c>
+      <c r="BD14" s="54">
+        <v>27674.122635126769</v>
+      </c>
     </row>
-    <row r="15" spans="1:55">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>99</v>
       </c>
@@ -19024,11 +19066,14 @@
       <c r="BB15" s="28">
         <v>46479.453987895853</v>
       </c>
-      <c r="BC15" s="56">
+      <c r="BC15" s="54">
         <v>44033.739364583002</v>
       </c>
+      <c r="BD15" s="54">
+        <v>45654.841883490524</v>
+      </c>
     </row>
-    <row r="16" spans="1:55">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -19191,11 +19236,14 @@
       <c r="BB16" s="28">
         <v>24952.473850869548</v>
       </c>
-      <c r="BC16" s="56">
+      <c r="BC16" s="54">
         <v>23616.98740361477</v>
       </c>
+      <c r="BD16" s="54">
+        <v>24304.043803267814</v>
+      </c>
     </row>
-    <row r="17" spans="1:55">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -19358,11 +19406,14 @@
       <c r="BB17" s="28">
         <v>30909.911403073944</v>
       </c>
-      <c r="BC17" s="56">
+      <c r="BC17" s="54">
         <v>28570.684239854159</v>
       </c>
+      <c r="BD17" s="54">
+        <v>28565.177524536717</v>
+      </c>
     </row>
-    <row r="18" spans="1:55">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -19525,11 +19576,14 @@
       <c r="BB18" s="28">
         <v>26144.953556607848</v>
       </c>
-      <c r="BC18" s="56">
+      <c r="BC18" s="54">
         <v>25006.093563234783</v>
       </c>
+      <c r="BD18" s="54">
+        <v>25885.895878571653</v>
+      </c>
     </row>
-    <row r="19" spans="1:55">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -19692,11 +19746,14 @@
       <c r="BB19" s="28">
         <v>25299.825539030266</v>
       </c>
-      <c r="BC19" s="56">
+      <c r="BC19" s="54">
         <v>23733.000129903721</v>
       </c>
+      <c r="BD19" s="54">
+        <v>23610.86379532265</v>
+      </c>
     </row>
-    <row r="20" spans="1:55">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -19859,11 +19916,14 @@
       <c r="BB20" s="28">
         <v>27704.16397870623</v>
       </c>
-      <c r="BC20" s="56">
+      <c r="BC20" s="54">
         <v>25755.629702890903</v>
       </c>
+      <c r="BD20" s="54">
+        <v>27155.488981381644</v>
+      </c>
     </row>
-    <row r="21" spans="1:55">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -20026,11 +20086,14 @@
       <c r="BB21" s="28">
         <v>31039.746984540296</v>
       </c>
-      <c r="BC21" s="56">
+      <c r="BC21" s="54">
         <v>30535.250127745061</v>
       </c>
+      <c r="BD21" s="54">
+        <v>31183.245413320794</v>
+      </c>
     </row>
-    <row r="22" spans="1:55">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -20193,11 +20256,14 @@
       <c r="BB22" s="28">
         <v>31069.218104372274</v>
       </c>
-      <c r="BC22" s="56">
+      <c r="BC22" s="54">
         <v>28814.80587263083</v>
       </c>
+      <c r="BD22" s="54">
+        <v>29458.277438410081</v>
+      </c>
     </row>
-    <row r="23" spans="1:55">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>93</v>
       </c>
@@ -20360,11 +20426,14 @@
       <c r="BB23" s="28">
         <v>76916.37314439725</v>
       </c>
-      <c r="BC23" s="56">
+      <c r="BC23" s="54">
         <v>67677.77981857222</v>
       </c>
+      <c r="BD23" s="54">
+        <v>69521.709462201616</v>
+      </c>
     </row>
-    <row r="24" spans="1:55">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -20527,11 +20596,14 @@
       <c r="BB24" s="28">
         <v>35264.912704266826</v>
       </c>
-      <c r="BC24" s="56">
+      <c r="BC24" s="54">
         <v>31331.533303265394</v>
       </c>
+      <c r="BD24" s="54">
+        <v>33227.272579679608</v>
+      </c>
     </row>
-    <row r="25" spans="1:55">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -20694,11 +20766,14 @@
       <c r="BB25" s="28">
         <v>49613.28561296931</v>
       </c>
-      <c r="BC25" s="56">
+      <c r="BC25" s="54">
         <v>44142.438395118908</v>
       </c>
+      <c r="BD25" s="54">
+        <v>42992.798212951457</v>
+      </c>
     </row>
-    <row r="26" spans="1:55">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -20861,11 +20936,14 @@
       <c r="BB26" s="28">
         <v>46123.324995913681</v>
       </c>
-      <c r="BC26" s="56">
+      <c r="BC26" s="54">
         <v>40172.639000197778</v>
       </c>
+      <c r="BD26" s="54">
+        <v>41770.939654026988</v>
+      </c>
     </row>
-    <row r="27" spans="1:55">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>116</v>
       </c>
@@ -21028,11 +21106,14 @@
       <c r="BB27" s="28">
         <v>84417.983001376619</v>
       </c>
-      <c r="BC27" s="56">
+      <c r="BC27" s="54">
         <v>69106.291067114551</v>
       </c>
+      <c r="BD27" s="54">
+        <v>68852.259476932624</v>
+      </c>
     </row>
-    <row r="28" spans="1:55">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -21195,11 +21276,14 @@
       <c r="BB28" s="28">
         <v>31055.483975470459</v>
       </c>
-      <c r="BC28" s="56">
+      <c r="BC28" s="54">
         <v>31022.923253815425</v>
       </c>
+      <c r="BD28" s="54">
+        <v>31106.756130334117</v>
+      </c>
     </row>
-    <row r="29" spans="1:55">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -21362,11 +21446,14 @@
       <c r="BB29" s="28">
         <v>31157.079751032612</v>
       </c>
-      <c r="BC29" s="56">
+      <c r="BC29" s="54">
         <v>30543.91762365873</v>
       </c>
+      <c r="BD29" s="54">
+        <v>30627.738121784118</v>
+      </c>
     </row>
-    <row r="30" spans="1:55">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -21529,11 +21616,14 @@
       <c r="BB30" s="28">
         <v>38795.566787477081</v>
       </c>
-      <c r="BC30" s="56">
+      <c r="BC30" s="54">
         <v>38347.715265716593</v>
       </c>
+      <c r="BD30" s="54">
+        <v>38068.805926031288</v>
+      </c>
     </row>
-    <row r="31" spans="1:55">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -21696,11 +21786,14 @@
       <c r="BB31" s="28">
         <v>56704.402775866198</v>
       </c>
-      <c r="BC31" s="56">
+      <c r="BC31" s="54">
         <v>45326.609005029866</v>
       </c>
+      <c r="BD31" s="54">
+        <v>48115.8147149496</v>
+      </c>
     </row>
-    <row r="32" spans="1:55">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -21863,11 +21956,14 @@
       <c r="BB32" s="28">
         <v>29380.257664137305</v>
       </c>
-      <c r="BC32" s="56">
+      <c r="BC32" s="54">
         <v>29020.556975314244</v>
       </c>
+      <c r="BD32" s="54">
+        <v>29049.412248544344</v>
+      </c>
     </row>
-    <row r="33" spans="1:55">
+    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
@@ -22030,11 +22126,14 @@
       <c r="BB33" s="28">
         <v>24330.602452640145</v>
       </c>
-      <c r="BC33" s="56">
+      <c r="BC33" s="54">
         <v>22160.056407309192</v>
       </c>
+      <c r="BD33" s="54">
+        <v>22605.929962540235</v>
+      </c>
     </row>
-    <row r="34" spans="1:55">
+    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
@@ -22197,11 +22296,14 @@
       <c r="BB34" s="28">
         <v>52269.405080487537</v>
       </c>
-      <c r="BC34" s="56">
+      <c r="BC34" s="54">
         <v>51571.410311259999</v>
       </c>
+      <c r="BD34" s="54">
+        <v>52604.936339565334</v>
+      </c>
     </row>
-    <row r="35" spans="1:55">
+    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
@@ -22364,11 +22466,14 @@
       <c r="BB35" s="28">
         <v>24773.005620148619</v>
       </c>
-      <c r="BC35" s="56">
+      <c r="BC35" s="54">
         <v>22766.083866226458</v>
       </c>
+      <c r="BD35" s="54">
+        <v>23601.397743454923</v>
+      </c>
     </row>
-    <row r="36" spans="1:55">
+    <row r="36" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>38</v>
       </c>
@@ -22531,11 +22636,14 @@
       <c r="BB36" s="28">
         <v>24550.862695954635</v>
       </c>
-      <c r="BC36" s="56">
+      <c r="BC36" s="54">
         <v>22326.442577940539</v>
       </c>
+      <c r="BD36" s="54">
+        <v>22593.822161461052</v>
+      </c>
     </row>
-    <row r="37" spans="1:55">
+    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>104</v>
       </c>
@@ -22650,11 +22758,14 @@
       <c r="BB37" s="28">
         <v>26322.917905137339</v>
       </c>
-      <c r="BC37" s="56">
+      <c r="BC37" s="54">
         <v>24775.072162054126</v>
       </c>
+      <c r="BD37" s="54">
+        <v>26384.556377336619</v>
+      </c>
     </row>
-    <row r="38" spans="1:55">
+    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>39</v>
       </c>
@@ -22817,11 +22928,14 @@
       <c r="BB38" s="28">
         <v>31297.373997167593</v>
       </c>
-      <c r="BC38" s="56">
+      <c r="BC38" s="54">
         <v>30309.722334383729</v>
       </c>
+      <c r="BD38" s="54">
+        <v>30591.747668706073</v>
+      </c>
     </row>
-    <row r="39" spans="1:55">
+    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>40</v>
       </c>
@@ -22984,11 +23098,14 @@
       <c r="BB39" s="28">
         <v>28013.319871262709</v>
       </c>
-      <c r="BC39" s="56">
+      <c r="BC39" s="54">
         <v>29859.505909547875</v>
       </c>
+      <c r="BD39" s="54">
+        <v>28673.857645272921</v>
+      </c>
     </row>
-    <row r="40" spans="1:55">
+    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>41</v>
       </c>
@@ -23151,11 +23268,14 @@
       <c r="BB40" s="28">
         <v>28620.572560871165</v>
       </c>
-      <c r="BC40" s="56">
+      <c r="BC40" s="54">
         <v>27201.964330004263</v>
       </c>
+      <c r="BD40" s="54">
+        <v>27391.272344773897</v>
+      </c>
     </row>
-    <row r="41" spans="1:55">
+    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
@@ -23318,11 +23438,14 @@
       <c r="BB41" s="28">
         <v>28255.942974566231</v>
       </c>
-      <c r="BC41" s="56">
+      <c r="BC41" s="54">
         <v>27063.966643429481</v>
       </c>
+      <c r="BD41" s="54">
+        <v>27657.160692898986</v>
+      </c>
     </row>
-    <row r="42" spans="1:55">
+    <row r="42" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>105</v>
       </c>
@@ -23437,11 +23560,14 @@
       <c r="BB42" s="28">
         <v>25651.784032656538</v>
       </c>
-      <c r="BC42" s="56">
+      <c r="BC42" s="54">
         <v>25180.455681059873</v>
       </c>
+      <c r="BD42" s="54">
+        <v>27069.630730784182</v>
+      </c>
     </row>
-    <row r="43" spans="1:55">
+    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>44</v>
       </c>
@@ -23604,11 +23730,14 @@
       <c r="BB43" s="28">
         <v>22382.716464128243</v>
       </c>
-      <c r="BC43" s="56">
+      <c r="BC43" s="54">
         <v>20519.663944495354</v>
       </c>
+      <c r="BD43" s="54">
+        <v>23004.755278561999</v>
+      </c>
     </row>
-    <row r="44" spans="1:55">
+    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>45</v>
       </c>
@@ -23771,11 +23900,14 @@
       <c r="BB44" s="28">
         <v>22759.53240639151</v>
       </c>
-      <c r="BC44" s="56">
+      <c r="BC44" s="54">
         <v>20391.156999696326</v>
       </c>
+      <c r="BD44" s="54">
+        <v>21431.166130424546</v>
+      </c>
     </row>
-    <row r="45" spans="1:55">
+    <row r="45" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>46</v>
       </c>
@@ -23938,11 +24070,14 @@
       <c r="BB45" s="28">
         <v>21219.350840175441</v>
       </c>
-      <c r="BC45" s="56">
+      <c r="BC45" s="54">
         <v>20980.180668125238</v>
       </c>
+      <c r="BD45" s="54">
+        <v>21264.232758649287</v>
+      </c>
     </row>
-    <row r="46" spans="1:55">
+    <row r="46" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
@@ -24105,11 +24240,14 @@
       <c r="BB46" s="28">
         <v>22836.307281251131</v>
       </c>
-      <c r="BC46" s="56">
+      <c r="BC46" s="54">
         <v>21166.141284550111</v>
       </c>
+      <c r="BD46" s="54">
+        <v>22010.226526353239</v>
+      </c>
     </row>
-    <row r="47" spans="1:55">
+    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>48</v>
       </c>
@@ -24272,11 +24410,14 @@
       <c r="BB47" s="28">
         <v>23598.111393491828</v>
       </c>
-      <c r="BC47" s="56">
+      <c r="BC47" s="54">
         <v>21189.073615370467</v>
       </c>
+      <c r="BD47" s="54">
+        <v>23133.6800374249</v>
+      </c>
     </row>
-    <row r="48" spans="1:55">
+    <row r="48" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>49</v>
       </c>
@@ -24439,11 +24580,14 @@
       <c r="BB48" s="28">
         <v>22873.65337707445</v>
       </c>
-      <c r="BC48" s="56">
+      <c r="BC48" s="54">
         <v>21124.840577996816</v>
       </c>
+      <c r="BD48" s="54">
+        <v>24168.238610299853</v>
+      </c>
     </row>
-    <row r="49" spans="1:55">
+    <row r="49" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>50</v>
       </c>
@@ -24606,11 +24750,14 @@
       <c r="BB49" s="28">
         <v>25990.726407639901</v>
       </c>
-      <c r="BC49" s="56">
+      <c r="BC49" s="54">
         <v>26773.36411412157</v>
       </c>
+      <c r="BD49" s="54">
+        <v>26786.972763775229</v>
+      </c>
     </row>
-    <row r="50" spans="1:55">
+    <row r="50" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>51</v>
       </c>
@@ -24773,11 +24920,14 @@
       <c r="BB50" s="28">
         <v>31982.674714937031</v>
       </c>
-      <c r="BC50" s="56">
+      <c r="BC50" s="54">
         <v>30186.961374769799</v>
       </c>
+      <c r="BD50" s="54">
+        <v>29866.455889692323</v>
+      </c>
     </row>
-    <row r="51" spans="1:55">
+    <row r="51" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>52</v>
       </c>
@@ -24940,11 +25090,14 @@
       <c r="BB51" s="28">
         <v>28831.50027179551</v>
       </c>
-      <c r="BC51" s="56">
+      <c r="BC51" s="54">
         <v>24736.645483346212</v>
       </c>
+      <c r="BD51" s="54">
+        <v>25234.811841883373</v>
+      </c>
     </row>
-    <row r="52" spans="1:55">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>53</v>
       </c>
@@ -25107,11 +25260,14 @@
       <c r="BB52" s="28">
         <v>24726.518144210622</v>
       </c>
-      <c r="BC52" s="56">
+      <c r="BC52" s="54">
         <v>24863.740230533585</v>
       </c>
+      <c r="BD52" s="54">
+        <v>25358.057228093869</v>
+      </c>
     </row>
-    <row r="53" spans="1:55">
+    <row r="53" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>54</v>
       </c>
@@ -25274,11 +25430,14 @@
       <c r="BB53" s="28">
         <v>33376.791867937573</v>
       </c>
-      <c r="BC53" s="56">
+      <c r="BC53" s="54">
         <v>31448.459784798903</v>
       </c>
+      <c r="BD53" s="54">
+        <v>31486.095972331252</v>
+      </c>
     </row>
-    <row r="54" spans="1:55">
+    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
@@ -25441,11 +25600,14 @@
       <c r="BB54" s="28">
         <v>30133.612635619738</v>
       </c>
-      <c r="BC54" s="56">
+      <c r="BC54" s="54">
         <v>28239.013233921498</v>
       </c>
+      <c r="BD54" s="54">
+        <v>29583.465327745944</v>
+      </c>
     </row>
-    <row r="55" spans="1:55">
+    <row r="55" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>56</v>
       </c>
@@ -25608,11 +25770,14 @@
       <c r="BB55" s="28">
         <v>24743.448635262757</v>
       </c>
-      <c r="BC55" s="56">
+      <c r="BC55" s="54">
         <v>23784.788541061429</v>
       </c>
+      <c r="BD55" s="54">
+        <v>24273.478530610799</v>
+      </c>
     </row>
-    <row r="56" spans="1:55">
+    <row r="56" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>57</v>
       </c>
@@ -25775,11 +25940,14 @@
       <c r="BB56" s="28">
         <v>32767.432414290754</v>
       </c>
-      <c r="BC56" s="56">
+      <c r="BC56" s="54">
         <v>31026.640395313436</v>
       </c>
+      <c r="BD56" s="54">
+        <v>31420.183892129357</v>
+      </c>
     </row>
-    <row r="57" spans="1:55">
+    <row r="57" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
@@ -25942,11 +26110,14 @@
       <c r="BB57" s="28">
         <v>24899.786439222935</v>
       </c>
-      <c r="BC57" s="56">
+      <c r="BC57" s="54">
         <v>24098.166944212277</v>
       </c>
+      <c r="BD57" s="54">
+        <v>24714.772280032728</v>
+      </c>
     </row>
-    <row r="58" spans="1:55">
+    <row r="58" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>59</v>
       </c>
@@ -26109,11 +26280,14 @@
       <c r="BB58" s="28">
         <v>30864.958277951737</v>
       </c>
-      <c r="BC58" s="56">
+      <c r="BC58" s="54">
         <v>29199.308047980998</v>
       </c>
+      <c r="BD58" s="54">
+        <v>29303.392197477933</v>
+      </c>
     </row>
-    <row r="59" spans="1:55">
+    <row r="59" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>60</v>
       </c>
@@ -26276,11 +26450,14 @@
       <c r="BB59" s="28">
         <v>29285.458798034837</v>
       </c>
-      <c r="BC59" s="56">
+      <c r="BC59" s="54">
         <v>27129.494749659803</v>
       </c>
+      <c r="BD59" s="54">
+        <v>27225.573516255059</v>
+      </c>
     </row>
-    <row r="60" spans="1:55">
+    <row r="60" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>61</v>
       </c>
@@ -26443,11 +26620,14 @@
       <c r="BB60" s="28">
         <v>27046.929158461433</v>
       </c>
-      <c r="BC60" s="56">
+      <c r="BC60" s="54">
         <v>27487.271702085389</v>
       </c>
+      <c r="BD60" s="54">
+        <v>26297.44925076174</v>
+      </c>
     </row>
-    <row r="61" spans="1:55">
+    <row r="61" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>62</v>
       </c>
@@ -26610,11 +26790,14 @@
       <c r="BB61" s="28">
         <v>32259.986146209067</v>
       </c>
-      <c r="BC61" s="56">
+      <c r="BC61" s="54">
         <v>29065.31894849813</v>
       </c>
+      <c r="BD61" s="54">
+        <v>29566.701110124675</v>
+      </c>
     </row>
-    <row r="62" spans="1:55">
+    <row r="62" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>63</v>
       </c>
@@ -26777,11 +26960,14 @@
       <c r="BB62" s="28">
         <v>25069.776674149522</v>
       </c>
-      <c r="BC62" s="56">
+      <c r="BC62" s="54">
         <v>23979.717674587384</v>
       </c>
+      <c r="BD62" s="54">
+        <v>24183.366626290535</v>
+      </c>
     </row>
-    <row r="63" spans="1:55">
+    <row r="63" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>64</v>
       </c>
@@ -26944,11 +27130,14 @@
       <c r="BB63" s="28">
         <v>26254.790438381904</v>
       </c>
-      <c r="BC63" s="56">
+      <c r="BC63" s="54">
         <v>25146.644247743821</v>
       </c>
+      <c r="BD63" s="54">
+        <v>25692.930020757485</v>
+      </c>
     </row>
-    <row r="64" spans="1:55">
+    <row r="64" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>65</v>
       </c>
@@ -27111,11 +27300,14 @@
       <c r="BB64" s="28">
         <v>26561.481176677411</v>
       </c>
-      <c r="BC64" s="56">
+      <c r="BC64" s="54">
         <v>25200.290364518576</v>
       </c>
+      <c r="BD64" s="54">
+        <v>25640.187131575749</v>
+      </c>
     </row>
-    <row r="65" spans="1:55">
+    <row r="65" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
@@ -27278,11 +27470,14 @@
       <c r="BB65" s="28">
         <v>35984.7743034753</v>
       </c>
-      <c r="BC65" s="56">
+      <c r="BC65" s="54">
         <v>32049.924003019612</v>
       </c>
+      <c r="BD65" s="54">
+        <v>32669.80844074249</v>
+      </c>
     </row>
-    <row r="66" spans="1:55">
+    <row r="66" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>67</v>
       </c>
@@ -27445,11 +27640,14 @@
       <c r="BB66" s="28">
         <v>72097.26554480374</v>
       </c>
-      <c r="BC66" s="56">
+      <c r="BC66" s="54">
         <v>59229.992404331904</v>
       </c>
+      <c r="BD66" s="54">
+        <v>61947.392928685847</v>
+      </c>
     </row>
-    <row r="67" spans="1:55">
+    <row r="67" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>115</v>
       </c>
@@ -27612,11 +27810,14 @@
       <c r="BB67" s="28">
         <v>74859.536050178853</v>
       </c>
-      <c r="BC67" s="56">
+      <c r="BC67" s="54">
         <v>59907.627423452781</v>
       </c>
+      <c r="BD67" s="54">
+        <v>67312.604484573909</v>
+      </c>
     </row>
-    <row r="68" spans="1:55">
+    <row r="68" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>114</v>
       </c>
@@ -27779,11 +27980,14 @@
       <c r="BB68" s="28">
         <v>105414.11581257809</v>
       </c>
-      <c r="BC68" s="56">
+      <c r="BC68" s="54">
         <v>83101.756504161327</v>
       </c>
+      <c r="BD68" s="54">
+        <v>82085.799337306365</v>
+      </c>
     </row>
-    <row r="69" spans="1:55">
+    <row r="69" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>68</v>
       </c>
@@ -27946,11 +28150,14 @@
       <c r="BB69" s="28">
         <v>32726.729288669299</v>
       </c>
-      <c r="BC69" s="56">
+      <c r="BC69" s="54">
         <v>30997.187587687593</v>
       </c>
+      <c r="BD69" s="54">
+        <v>31713.459848451854</v>
+      </c>
     </row>
-    <row r="70" spans="1:55">
+    <row r="70" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>69</v>
       </c>
@@ -28113,11 +28320,14 @@
       <c r="BB70" s="28">
         <v>26930.128984881208</v>
       </c>
-      <c r="BC70" s="56">
+      <c r="BC70" s="54">
         <v>23099.277005813456</v>
       </c>
+      <c r="BD70" s="54">
+        <v>26323.273045678896</v>
+      </c>
     </row>
-    <row r="71" spans="1:55">
+    <row r="71" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>70</v>
       </c>
@@ -28280,11 +28490,14 @@
       <c r="BB71" s="28">
         <v>32048.76956765963</v>
       </c>
-      <c r="BC71" s="56">
+      <c r="BC71" s="54">
         <v>28474.647193973371</v>
       </c>
+      <c r="BD71" s="54">
+        <v>30382.259774987244</v>
+      </c>
     </row>
-    <row r="72" spans="1:55">
+    <row r="72" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
@@ -28447,11 +28660,14 @@
       <c r="BB72" s="28">
         <v>33608.89850803477</v>
       </c>
-      <c r="BC72" s="56">
+      <c r="BC72" s="54">
         <v>24890.109183337496</v>
       </c>
+      <c r="BD72" s="54">
+        <v>28854.763630119422</v>
+      </c>
     </row>
-    <row r="73" spans="1:55">
+    <row r="73" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
@@ -28614,11 +28830,14 @@
       <c r="BB73" s="28">
         <v>34701.323923599492</v>
       </c>
-      <c r="BC73" s="56">
+      <c r="BC73" s="54">
         <v>32197.135848722639</v>
       </c>
+      <c r="BD73" s="54">
+        <v>33562.064547377573</v>
+      </c>
     </row>
-    <row r="74" spans="1:55">
+    <row r="74" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>73</v>
       </c>
@@ -28781,11 +29000,14 @@
       <c r="BB74" s="28">
         <v>22503.840954751162</v>
       </c>
-      <c r="BC74" s="56">
+      <c r="BC74" s="54">
         <v>21912.615426888333</v>
       </c>
+      <c r="BD74" s="54">
+        <v>22885.323017414306</v>
+      </c>
     </row>
-    <row r="75" spans="1:55">
+    <row r="75" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>74</v>
       </c>
@@ -28948,11 +29170,14 @@
       <c r="BB75" s="28">
         <v>34904.879933233475</v>
       </c>
-      <c r="BC75" s="56">
+      <c r="BC75" s="54">
         <v>32075.385772884129</v>
       </c>
+      <c r="BD75" s="54">
+        <v>36085.383336159102</v>
+      </c>
     </row>
-    <row r="76" spans="1:55">
+    <row r="76" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
@@ -29115,11 +29340,14 @@
       <c r="BB76" s="28">
         <v>42610.08852592991</v>
       </c>
-      <c r="BC76" s="56">
+      <c r="BC76" s="54">
         <v>38092.063085868162</v>
       </c>
+      <c r="BD76" s="54">
+        <v>39743.181567233907</v>
+      </c>
     </row>
-    <row r="77" spans="1:55">
+    <row r="77" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
@@ -29282,11 +29510,14 @@
       <c r="BB77" s="28">
         <v>40527.592362838921</v>
       </c>
-      <c r="BC77" s="56">
+      <c r="BC77" s="54">
         <v>35449.404834341884</v>
       </c>
+      <c r="BD77" s="54">
+        <v>36386.056836820084</v>
+      </c>
     </row>
-    <row r="78" spans="1:55">
+    <row r="78" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
@@ -29449,11 +29680,14 @@
       <c r="BB78" s="28">
         <v>33700.546045289797</v>
       </c>
-      <c r="BC78" s="56">
+      <c r="BC78" s="54">
         <v>32343.564028304194</v>
       </c>
+      <c r="BD78" s="54">
+        <v>31565.395481961612</v>
+      </c>
     </row>
-    <row r="79" spans="1:55">
+    <row r="79" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -29616,11 +29850,14 @@
       <c r="BB79" s="28">
         <v>33417.030856990175</v>
       </c>
-      <c r="BC79" s="56">
+      <c r="BC79" s="54">
         <v>30776.895181936437</v>
       </c>
+      <c r="BD79" s="54">
+        <v>32089.538505475361</v>
+      </c>
     </row>
-    <row r="80" spans="1:55">
+    <row r="80" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
@@ -29783,11 +30020,14 @@
       <c r="BB80" s="28">
         <v>30914.225721762774</v>
       </c>
-      <c r="BC80" s="56">
+      <c r="BC80" s="54">
         <v>28345.226795388931</v>
       </c>
+      <c r="BD80" s="54">
+        <v>29818.264054660547</v>
+      </c>
     </row>
-    <row r="81" spans="1:55">
+    <row r="81" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
@@ -29950,11 +30190,14 @@
       <c r="BB81" s="28">
         <v>43232.331744922565</v>
       </c>
-      <c r="BC81" s="56">
+      <c r="BC81" s="54">
         <v>37351.421920854133</v>
       </c>
+      <c r="BD81" s="54">
+        <v>36840.363404314412</v>
+      </c>
     </row>
-    <row r="82" spans="1:55">
+    <row r="82" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>82</v>
       </c>
@@ -30117,11 +30360,14 @@
       <c r="BB82" s="28">
         <v>68590.068770599188</v>
       </c>
-      <c r="BC82" s="56">
+      <c r="BC82" s="54">
         <v>51825.852745958124</v>
       </c>
+      <c r="BD82" s="54">
+        <v>57588.898427887987</v>
+      </c>
     </row>
-    <row r="83" spans="1:55">
+    <row r="83" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>83</v>
       </c>
@@ -30284,11 +30530,14 @@
       <c r="BB83" s="28">
         <v>77043.251535660063</v>
       </c>
-      <c r="BC83" s="56">
+      <c r="BC83" s="54">
         <v>63761.459508414191</v>
       </c>
+      <c r="BD83" s="54">
+        <v>65100.008141676924</v>
+      </c>
     </row>
-    <row r="84" spans="1:55">
+    <row r="84" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>84</v>
       </c>
@@ -30451,11 +30700,14 @@
       <c r="BB84" s="28">
         <v>38986.146997387259</v>
       </c>
-      <c r="BC84" s="56">
+      <c r="BC84" s="54">
         <v>35441.558733805839</v>
       </c>
+      <c r="BD84" s="54">
+        <v>36909.43104089579</v>
+      </c>
     </row>
-    <row r="85" spans="1:55">
+    <row r="85" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>85</v>
       </c>
@@ -30618,11 +30870,14 @@
       <c r="BB85" s="28">
         <v>49014.703383520296</v>
       </c>
-      <c r="BC85" s="56">
+      <c r="BC85" s="54">
         <v>38869.444527199135</v>
       </c>
+      <c r="BD85" s="54">
+        <v>40937.795225341761</v>
+      </c>
     </row>
-    <row r="86" spans="1:55">
+    <row r="86" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>86</v>
       </c>
@@ -30785,11 +31040,14 @@
       <c r="BB86" s="28">
         <v>37521.953675837278</v>
       </c>
-      <c r="BC86" s="56">
+      <c r="BC86" s="54">
         <v>36190.327023923237</v>
       </c>
+      <c r="BD86" s="54">
+        <v>37324.0597580256</v>
+      </c>
     </row>
-    <row r="87" spans="1:55">
+    <row r="87" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>87</v>
       </c>
@@ -30952,11 +31210,14 @@
       <c r="BB87" s="28">
         <v>79958.651157946748</v>
       </c>
-      <c r="BC87" s="56">
+      <c r="BC87" s="54">
         <v>67693.961549808999</v>
       </c>
+      <c r="BD87" s="54">
+        <v>74712.097480850061</v>
+      </c>
     </row>
-    <row r="88" spans="1:55">
+    <row r="88" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>88</v>
       </c>
@@ -31119,11 +31380,14 @@
       <c r="BB88" s="28">
         <v>70052.393772833093</v>
       </c>
-      <c r="BC88" s="56">
+      <c r="BC88" s="54">
         <v>66616.33896611497</v>
       </c>
+      <c r="BD88" s="54">
+        <v>67073.863960133487</v>
+      </c>
     </row>
-    <row r="89" spans="1:55">
+    <row r="89" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>89</v>
       </c>
@@ -31286,11 +31550,14 @@
       <c r="BB89" s="28">
         <v>35517.898455346483</v>
       </c>
-      <c r="BC89" s="56">
+      <c r="BC89" s="54">
         <v>32016.023265662683</v>
       </c>
+      <c r="BD89" s="54">
+        <v>34058.955278697227</v>
+      </c>
     </row>
-    <row r="90" spans="1:55">
+    <row r="90" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>90</v>
       </c>
@@ -31453,16 +31720,19 @@
       <c r="BB90" s="28">
         <v>94997.137640590634</v>
       </c>
-      <c r="BC90" s="56">
+      <c r="BC90" s="54">
         <v>85138.87533398105</v>
       </c>
+      <c r="BD90" s="54">
+        <v>86423.797798248692</v>
+      </c>
     </row>
-    <row r="92" spans="1:55" ht="34.5">
+    <row r="92" spans="1:56" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A92" s="26" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="93" spans="1:55" ht="17.25">
+    <row r="93" spans="1:56" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A93" s="25"/>
     </row>
   </sheetData>
@@ -31476,12 +31746,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31489,12 +31759,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>